<commit_message>
Criação das dummies: Black Friday, Promocionado 25 e 50
</commit_message>
<xml_diff>
--- a/Forecast/Precos_para_previsoes.xlsx
+++ b/Forecast/Precos_para_previsoes.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Desktop\Projetos Git\Forecast vendas e elasticidade\Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB625A4-29F5-46D7-AA05-3485D6956D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B751B376-65DF-40CE-8FF8-31935389C4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="180" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Data</t>
   </si>
@@ -34,6 +45,12 @@
   </si>
   <si>
     <t>Preco</t>
+  </si>
+  <si>
+    <t>promocionado_25</t>
+  </si>
+  <si>
+    <t>Black_Friday</t>
   </si>
 </sst>
 </file>
@@ -352,18 +369,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -373,54 +388,84 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45914</v>
+        <v>45918</v>
       </c>
       <c r="B2">
         <v>7172</v>
       </c>
       <c r="C2">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>379.9</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45915</v>
+        <v>45919</v>
       </c>
       <c r="B3">
         <v>7172</v>
       </c>
       <c r="C3">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45916</v>
+        <v>45920</v>
       </c>
       <c r="B4">
         <v>7172</v>
       </c>
       <c r="C4">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>370.9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45917</v>
+        <v>45921</v>
       </c>
       <c r="B5">
         <v>7172</v>
       </c>
       <c r="C5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45918</v>
+        <v>45922</v>
       </c>
       <c r="B6">
         <v>7172</v>
@@ -428,41 +473,66 @@
       <c r="C6">
         <v>350</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45919</v>
+        <v>45923</v>
       </c>
       <c r="B7">
         <v>7172</v>
       </c>
       <c r="C7">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45920</v>
+        <v>45924</v>
       </c>
       <c r="B8">
         <v>7172</v>
       </c>
       <c r="C8">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45921</v>
+        <v>45925</v>
       </c>
       <c r="B9">
         <v>7172</v>
       </c>
       <c r="C9">
-        <v>360</v>
+        <v>380</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustes no modelo sarimax e tscv criação das novas funções de previsão arquivos de previsão ajuste nos gráficos da validação estatistica implementação dos novos cálculos de previsão e gráficos para comparar dados reais e das previsões.
</commit_message>
<xml_diff>
--- a/Forecast/Precos_para_previsoes.xlsx
+++ b/Forecast/Precos_para_previsoes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Desktop\Projetos Git\Forecast vendas e elasticidade\Forecast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.pcarvalho\Desktop\Git Repositórios\Forecast-vendas-e-elasticidade\Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B751B376-65DF-40CE-8FF8-31935389C4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906FD13B-65D0-49A7-A60C-CCBB71472D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-555" windowWidth="14400" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Data</t>
   </si>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Preco</t>
-  </si>
-  <si>
-    <t>promocionado_25</t>
-  </si>
-  <si>
-    <t>Black_Friday</t>
   </si>
 </sst>
 </file>
@@ -369,16 +363,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,14 +384,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45918</v>
       </c>
@@ -403,16 +393,10 @@
         <v>7172</v>
       </c>
       <c r="C2">
-        <v>379.9</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45919</v>
       </c>
@@ -422,14 +406,8 @@
       <c r="C3">
         <v>375</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45920</v>
       </c>
@@ -437,16 +415,10 @@
         <v>7172</v>
       </c>
       <c r="C4">
-        <v>370.9</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45921</v>
       </c>
@@ -454,16 +426,10 @@
         <v>7172</v>
       </c>
       <c r="C5">
-        <v>372</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45922</v>
       </c>
@@ -471,16 +437,10 @@
         <v>7172</v>
       </c>
       <c r="C6">
-        <v>350</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45923</v>
       </c>
@@ -488,16 +448,10 @@
         <v>7172</v>
       </c>
       <c r="C7">
-        <v>350</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45924</v>
       </c>
@@ -505,16 +459,10 @@
         <v>7172</v>
       </c>
       <c r="C8">
-        <v>300</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45925</v>
       </c>
@@ -522,13 +470,29 @@
         <v>7172</v>
       </c>
       <c r="C9">
-        <v>380</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45926</v>
+      </c>
+      <c r="B10">
+        <v>7172</v>
+      </c>
+      <c r="C10">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>45927</v>
+      </c>
+      <c r="B11">
+        <v>7172</v>
+      </c>
+      <c r="C11">
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da função pred_prox_30_dias
</commit_message>
<xml_diff>
--- a/Forecast/Precos_para_previsoes.xlsx
+++ b/Forecast/Precos_para_previsoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.pcarvalho\Desktop\Git Repositórios\Forecast-vendas-e-elasticidade\Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924026B6-2B31-4FE7-89EE-BDB215858DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105DC69-9C8E-4D10-8CF6-5964F2F8DB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-555" windowWidth="14400" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,7 +503,7 @@
         <v>7172</v>
       </c>
       <c r="C12">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -525,7 +525,7 @@
         <v>7172</v>
       </c>
       <c r="C14">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Mudança de SARIMAX para ARIMAX Ajuste nos modelos Criação da validação de modelos Criação da previsal total Adição de intercepto ao arima mudanças no readme
</commit_message>
<xml_diff>
--- a/Forecast/Precos_para_previsoes.xlsx
+++ b/Forecast/Precos_para_previsoes.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.pcarvalho\Desktop\Git Repositórios\Forecast-vendas-e-elasticidade\Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F66D2-FDA0-4785-A9B6-EFCBFB5AC33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9718771E-1DED-4495-81E1-A4DBFD9CB39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43650" yWindow="405" windowWidth="14400" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$60</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,9 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,311 +545,549 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>45918</v>
+        <v>45901</v>
       </c>
       <c r="B16">
         <v>10036</v>
       </c>
       <c r="C16">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>45919</v>
+        <v>45902</v>
       </c>
       <c r="B17">
         <v>10036</v>
       </c>
       <c r="C17">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>45920</v>
+        <v>45903</v>
       </c>
       <c r="B18">
         <v>10036</v>
       </c>
       <c r="C18">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>45921</v>
+        <v>45904</v>
       </c>
       <c r="B19">
         <v>10036</v>
       </c>
       <c r="C19">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>45922</v>
+        <v>45905</v>
       </c>
       <c r="B20">
         <v>10036</v>
       </c>
       <c r="C20">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>45923</v>
+        <v>45906</v>
       </c>
       <c r="B21">
         <v>10036</v>
       </c>
       <c r="C21">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>45924</v>
+        <v>45907</v>
       </c>
       <c r="B22">
         <v>10036</v>
       </c>
       <c r="C22">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>45925</v>
+        <v>45908</v>
       </c>
       <c r="B23">
         <v>10036</v>
       </c>
       <c r="C23">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>45926</v>
+        <v>45909</v>
       </c>
       <c r="B24">
         <v>10036</v>
       </c>
       <c r="C24">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>45927</v>
+        <v>45910</v>
       </c>
       <c r="B25">
         <v>10036</v>
       </c>
       <c r="C25">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>45928</v>
+        <v>45911</v>
       </c>
       <c r="B26">
         <v>10036</v>
       </c>
       <c r="C26">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>45929</v>
+        <v>45912</v>
       </c>
       <c r="B27">
         <v>10036</v>
       </c>
       <c r="C27">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>45930</v>
+        <v>45913</v>
       </c>
       <c r="B28">
         <v>10036</v>
       </c>
       <c r="C28">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>45931</v>
+        <v>45914</v>
       </c>
       <c r="B29">
         <v>10036</v>
       </c>
       <c r="C29">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>45918</v>
+        <v>45915</v>
       </c>
       <c r="B30">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C30">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>45919</v>
+        <v>45916</v>
       </c>
       <c r="B31">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C31">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>45920</v>
+        <v>45917</v>
       </c>
       <c r="B32">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C32">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>45921</v>
+        <v>45918</v>
       </c>
       <c r="B33">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C33">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>45922</v>
+        <v>45919</v>
       </c>
       <c r="B34">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C34">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>45923</v>
+        <v>45920</v>
       </c>
       <c r="B35">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C35">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>45924</v>
+        <v>45921</v>
       </c>
       <c r="B36">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C36">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>45925</v>
+        <v>45922</v>
       </c>
       <c r="B37">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C37">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>45926</v>
+        <v>45923</v>
       </c>
       <c r="B38">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C38">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>45927</v>
+        <v>45924</v>
       </c>
       <c r="B39">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C39">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>45928</v>
+        <v>45925</v>
       </c>
       <c r="B40">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C40">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>45929</v>
+        <v>45926</v>
       </c>
       <c r="B41">
-        <v>21120</v>
-      </c>
-      <c r="C41">
-        <v>56</v>
+        <v>10036</v>
+      </c>
+      <c r="C41" s="2">
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>45930</v>
+        <v>45927</v>
       </c>
       <c r="B42">
-        <v>21120</v>
+        <v>10036</v>
       </c>
       <c r="C42">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
+        <v>45928</v>
+      </c>
+      <c r="B43">
+        <v>10036</v>
+      </c>
+      <c r="C43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>45929</v>
+      </c>
+      <c r="B44">
+        <v>10036</v>
+      </c>
+      <c r="C44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B45">
+        <v>10036</v>
+      </c>
+      <c r="C45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
         <v>45931</v>
       </c>
-      <c r="B43">
-        <v>21120</v>
-      </c>
-      <c r="C43">
+      <c r="B46">
+        <v>10036</v>
+      </c>
+      <c r="C46">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>45918</v>
+      </c>
+      <c r="B47">
+        <v>21120</v>
+      </c>
+      <c r="C47">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>45919</v>
+      </c>
+      <c r="B48">
+        <v>21120</v>
+      </c>
+      <c r="C48">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>45920</v>
+      </c>
+      <c r="B49">
+        <v>21120</v>
+      </c>
+      <c r="C49">
         <v>60</v>
       </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>45921</v>
+      </c>
+      <c r="B50">
+        <v>21120</v>
+      </c>
+      <c r="C50">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>45922</v>
+      </c>
+      <c r="B51">
+        <v>21120</v>
+      </c>
+      <c r="C51">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>45923</v>
+      </c>
+      <c r="B52">
+        <v>21120</v>
+      </c>
+      <c r="C52">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>45924</v>
+      </c>
+      <c r="B53">
+        <v>21120</v>
+      </c>
+      <c r="C53">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>45925</v>
+      </c>
+      <c r="B54">
+        <v>21120</v>
+      </c>
+      <c r="C54">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>45926</v>
+      </c>
+      <c r="B55">
+        <v>21120</v>
+      </c>
+      <c r="C55">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>45927</v>
+      </c>
+      <c r="B56">
+        <v>21120</v>
+      </c>
+      <c r="C56">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>45928</v>
+      </c>
+      <c r="B57">
+        <v>21120</v>
+      </c>
+      <c r="C57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>45929</v>
+      </c>
+      <c r="B58">
+        <v>21120</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B59">
+        <v>21120</v>
+      </c>
+      <c r="C59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>45931</v>
+      </c>
+      <c r="B60">
+        <v>21120</v>
+      </c>
+      <c r="C60" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajuste nas funções de previsão para o pipeline Criação da célula de envio dos resultados ao Big Query
</commit_message>
<xml_diff>
--- a/Forecast/Precos_para_previsoes.xlsx
+++ b/Forecast/Precos_para_previsoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.pcarvalho\Desktop\Git Repositórios\Forecast-vendas-e-elasticidade\Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28F9238-4686-4394-AD49-03EC5D7E674B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C20EFE3-83B8-41D3-87BA-9A45968799F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$97</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -371,8 +371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1335,13 +1335,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>45931</v>
+        <v>45932</v>
       </c>
       <c r="B69">
-        <v>80625</v>
+        <v>21120</v>
       </c>
       <c r="C69">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -1349,13 +1349,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>45931</v>
+        <v>45933</v>
       </c>
       <c r="B70">
-        <v>77244</v>
+        <v>21120</v>
       </c>
       <c r="C70">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -1363,13 +1363,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>45931</v>
+        <v>45934</v>
       </c>
       <c r="B71">
-        <v>52251</v>
+        <v>21120</v>
       </c>
       <c r="C71">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -1377,372 +1377,97 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>45931</v>
+        <v>45935</v>
       </c>
       <c r="B72">
-        <v>71248</v>
+        <v>21120</v>
       </c>
       <c r="C72">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B73">
-        <v>9891</v>
-      </c>
-      <c r="C73">
-        <v>37</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
+      <c r="A73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B74">
-        <v>58407</v>
-      </c>
-      <c r="C74">
-        <v>21</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
+      <c r="A74" s="1"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B75">
-        <v>30717</v>
-      </c>
-      <c r="C75">
-        <v>59</v>
-      </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
+      <c r="A75" s="1"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B76">
-        <v>42891</v>
-      </c>
-      <c r="C76">
-        <v>30</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
+      <c r="A76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B77">
-        <v>36949</v>
-      </c>
-      <c r="C77">
-        <v>99</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
+      <c r="A77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B78">
-        <v>88308</v>
-      </c>
-      <c r="C78">
-        <v>30</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
+      <c r="A78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B79">
-        <v>81379</v>
-      </c>
-      <c r="C79">
-        <v>46</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
+      <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B80">
-        <v>77243</v>
-      </c>
-      <c r="C80">
-        <v>38</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B81">
-        <v>83626</v>
-      </c>
-      <c r="C81">
-        <v>724</v>
-      </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B82">
-        <v>34891</v>
-      </c>
-      <c r="C82">
-        <v>119</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B83">
-        <v>21120</v>
-      </c>
-      <c r="C83">
-        <v>57</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B84">
-        <v>80625</v>
-      </c>
-      <c r="C84">
-        <v>79</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B85">
-        <v>77244</v>
-      </c>
-      <c r="C85">
-        <v>75</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B86">
-        <v>52251</v>
-      </c>
-      <c r="C86">
-        <v>62</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B87">
-        <v>71248</v>
-      </c>
-      <c r="C87">
-        <v>88</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B88">
-        <v>9891</v>
-      </c>
-      <c r="C88">
-        <v>37</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B89">
-        <v>58407</v>
-      </c>
-      <c r="C89">
-        <v>21</v>
-      </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A90" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B90">
-        <v>30717</v>
-      </c>
-      <c r="C90">
-        <v>59</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B91">
-        <v>42891</v>
-      </c>
-      <c r="C91">
-        <v>30</v>
-      </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B92">
-        <v>36949</v>
-      </c>
-      <c r="C92">
-        <v>99</v>
-      </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B93">
-        <v>88308</v>
-      </c>
-      <c r="C93">
-        <v>30</v>
-      </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B94">
-        <v>81379</v>
-      </c>
-      <c r="C94">
-        <v>46</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B95">
-        <v>77243</v>
-      </c>
-      <c r="C95">
-        <v>38</v>
-      </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B96">
-        <v>83626</v>
-      </c>
-      <c r="C96">
-        <v>724</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B97">
-        <v>34891</v>
-      </c>
-      <c r="C97">
-        <v>119</v>
-      </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes finos no modelo de elasticidade e criação do modelo de VMD para o time de abastecimendo.
</commit_message>
<xml_diff>
--- a/Forecast/Precos_para_previsoes.xlsx
+++ b/Forecast/Precos_para_previsoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.pcarvalho\Desktop\Git Repositórios\Forecast-vendas-e-elasticidade\Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C20EFE3-83B8-41D3-87BA-9A45968799F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A262363-A258-4E15-BCDF-4C2D308B1CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -371,9 +371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -397,13 +395,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45918</v>
+        <v>45962</v>
       </c>
       <c r="B2">
         <v>7172</v>
       </c>
       <c r="C2">
-        <v>379</v>
+        <v>351</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -411,13 +409,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45919</v>
+        <v>45963</v>
       </c>
       <c r="B3">
         <v>7172</v>
       </c>
       <c r="C3">
-        <v>375</v>
+        <v>347</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -425,13 +423,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>45920</v>
+        <v>45964</v>
       </c>
       <c r="B4">
         <v>7172</v>
       </c>
       <c r="C4">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -439,13 +437,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45921</v>
+        <v>45965</v>
       </c>
       <c r="B5">
         <v>7172</v>
       </c>
       <c r="C5">
-        <v>369</v>
+        <v>336</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -453,13 +451,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45922</v>
+        <v>45966</v>
       </c>
       <c r="B6">
         <v>7172</v>
       </c>
       <c r="C6">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -467,13 +465,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45923</v>
+        <v>45967</v>
       </c>
       <c r="B7">
         <v>7172</v>
       </c>
       <c r="C7">
-        <v>372</v>
+        <v>320</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -481,27 +479,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45924</v>
+        <v>45968</v>
       </c>
       <c r="B8">
         <v>7172</v>
       </c>
       <c r="C8">
-        <v>369</v>
+        <v>287</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45925</v>
+        <v>45969</v>
       </c>
       <c r="B9">
         <v>7172</v>
       </c>
       <c r="C9">
-        <v>366</v>
+        <v>304</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -509,13 +507,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45926</v>
+        <v>45970</v>
       </c>
       <c r="B10">
         <v>7172</v>
       </c>
       <c r="C10">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -523,13 +521,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45927</v>
+        <v>45971</v>
       </c>
       <c r="B11">
         <v>7172</v>
       </c>
       <c r="C11">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -537,13 +535,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45928</v>
+        <v>45972</v>
       </c>
       <c r="B12">
         <v>7172</v>
       </c>
       <c r="C12">
-        <v>360</v>
+        <v>329</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -551,13 +549,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45929</v>
+        <v>45973</v>
       </c>
       <c r="B13">
         <v>7172</v>
       </c>
       <c r="C13">
-        <v>360</v>
+        <v>329</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -565,13 +563,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45930</v>
+        <v>45974</v>
       </c>
       <c r="B14">
         <v>7172</v>
       </c>
       <c r="C14">
-        <v>369</v>
+        <v>288</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -579,13 +577,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>45931</v>
+        <v>45975</v>
       </c>
       <c r="B15">
         <v>7172</v>
       </c>
       <c r="C15">
-        <v>369</v>
+        <v>317</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -593,49 +591,49 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>45932</v>
+        <v>45976</v>
       </c>
       <c r="B16">
         <v>7172</v>
       </c>
       <c r="C16">
-        <v>299</v>
+        <v>376</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>45933</v>
+        <v>45977</v>
       </c>
       <c r="B17">
         <v>7172</v>
       </c>
       <c r="C17">
-        <v>295</v>
+        <v>376</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>45934</v>
+        <v>45978</v>
       </c>
       <c r="B18">
         <v>7172</v>
       </c>
       <c r="C18">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>45935</v>
+        <v>45979</v>
       </c>
       <c r="B19">
         <v>7172</v>

</xml_diff>